<commit_message>
update the tc function
</commit_message>
<xml_diff>
--- a/01_Dataset_Cleaned/MultiTaskModel_NiFe_CrMoTi_TC_wt_pct.xlsx
+++ b/01_Dataset_Cleaned/MultiTaskModel_NiFe_CrMoTi_TC_wt_pct.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -462,7 +462,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.1</v>
+        <v>26.86666666666667</v>
       </c>
       <c r="B2" t="n">
         <v>0.1</v>
@@ -474,12 +474,12 @@
         <v>0.1</v>
       </c>
       <c r="E2" t="n">
-        <v>99.60000000000002</v>
+        <v>72.83333333333333</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2.533333333333333</v>
+        <v>29.3</v>
       </c>
       <c r="B3" t="n">
         <v>0.1</v>
@@ -491,12 +491,12 @@
         <v>0.1</v>
       </c>
       <c r="E3" t="n">
-        <v>97.16666666666669</v>
+        <v>70.40000000000001</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>4.966666666666667</v>
+        <v>31.73333333333333</v>
       </c>
       <c r="B4" t="n">
         <v>0.1</v>
@@ -508,12 +508,12 @@
         <v>0.1</v>
       </c>
       <c r="E4" t="n">
-        <v>94.73333333333335</v>
+        <v>67.96666666666667</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>7.399999999999999</v>
+        <v>34.16666666666666</v>
       </c>
       <c r="B5" t="n">
         <v>0.1</v>
@@ -525,12 +525,12 @@
         <v>0.1</v>
       </c>
       <c r="E5" t="n">
-        <v>92.30000000000001</v>
+        <v>65.53333333333333</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>9.833333333333332</v>
+        <v>36.6</v>
       </c>
       <c r="B6" t="n">
         <v>0.1</v>
@@ -542,12 +542,12 @@
         <v>0.1</v>
       </c>
       <c r="E6" t="n">
-        <v>89.86666666666669</v>
+        <v>63.09999999999999</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>12.26666666666667</v>
+        <v>39.03333333333333</v>
       </c>
       <c r="B7" t="n">
         <v>0.1</v>
@@ -559,12 +559,12 @@
         <v>0.1</v>
       </c>
       <c r="E7" t="n">
-        <v>87.43333333333335</v>
+        <v>60.66666666666666</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>14.7</v>
+        <v>41.46666666666666</v>
       </c>
       <c r="B8" t="n">
         <v>0.1</v>
@@ -576,12 +576,12 @@
         <v>0.1</v>
       </c>
       <c r="E8" t="n">
-        <v>85.00000000000001</v>
+        <v>58.23333333333333</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>17.13333333333333</v>
+        <v>43.89999999999999</v>
       </c>
       <c r="B9" t="n">
         <v>0.1</v>
@@ -593,12 +593,12 @@
         <v>0.1</v>
       </c>
       <c r="E9" t="n">
-        <v>82.56666666666669</v>
+        <v>55.8</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>19.56666666666667</v>
+        <v>46.33333333333333</v>
       </c>
       <c r="B10" t="n">
         <v>0.1</v>
@@ -610,12 +610,12 @@
         <v>0.1</v>
       </c>
       <c r="E10" t="n">
-        <v>80.13333333333335</v>
+        <v>53.36666666666667</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>22</v>
+        <v>48.76666666666667</v>
       </c>
       <c r="B11" t="n">
         <v>0.1</v>
@@ -627,12 +627,12 @@
         <v>0.1</v>
       </c>
       <c r="E11" t="n">
-        <v>77.70000000000002</v>
+        <v>50.93333333333333</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>24.43333333333333</v>
+        <v>51.2</v>
       </c>
       <c r="B12" t="n">
         <v>0.1</v>
@@ -644,12 +644,12 @@
         <v>0.1</v>
       </c>
       <c r="E12" t="n">
-        <v>75.26666666666668</v>
+        <v>48.49999999999999</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>26.86666666666667</v>
+        <v>53.63333333333333</v>
       </c>
       <c r="B13" t="n">
         <v>0.1</v>
@@ -661,12 +661,12 @@
         <v>0.1</v>
       </c>
       <c r="E13" t="n">
-        <v>72.83333333333334</v>
+        <v>46.06666666666666</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>29.3</v>
+        <v>56.06666666666666</v>
       </c>
       <c r="B14" t="n">
         <v>0.1</v>
@@ -678,12 +678,12 @@
         <v>0.1</v>
       </c>
       <c r="E14" t="n">
-        <v>70.40000000000002</v>
+        <v>43.63333333333333</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>31.73333333333333</v>
+        <v>58.5</v>
       </c>
       <c r="B15" t="n">
         <v>0.1</v>
@@ -695,12 +695,12 @@
         <v>0.1</v>
       </c>
       <c r="E15" t="n">
-        <v>67.96666666666668</v>
+        <v>41.2</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>34.16666666666666</v>
+        <v>60.93333333333333</v>
       </c>
       <c r="B16" t="n">
         <v>0.1</v>
@@ -712,12 +712,12 @@
         <v>0.1</v>
       </c>
       <c r="E16" t="n">
-        <v>65.53333333333336</v>
+        <v>38.76666666666667</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>36.6</v>
+        <v>63.36666666666666</v>
       </c>
       <c r="B17" t="n">
         <v>0.1</v>
@@ -729,12 +729,12 @@
         <v>0.1</v>
       </c>
       <c r="E17" t="n">
-        <v>63.09999999999999</v>
+        <v>36.33333333333334</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>39.03333333333333</v>
+        <v>65.8</v>
       </c>
       <c r="B18" t="n">
         <v>0.1</v>
@@ -746,12 +746,12 @@
         <v>0.1</v>
       </c>
       <c r="E18" t="n">
-        <v>60.66666666666666</v>
+        <v>33.90000000000002</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>41.46666666666666</v>
+        <v>68.23333333333333</v>
       </c>
       <c r="B19" t="n">
         <v>0.1</v>
@@ -763,12 +763,12 @@
         <v>0.1</v>
       </c>
       <c r="E19" t="n">
-        <v>58.23333333333333</v>
+        <v>31.46666666666668</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>43.89999999999999</v>
+        <v>70.66666666666667</v>
       </c>
       <c r="B20" t="n">
         <v>0.1</v>
@@ -780,12 +780,12 @@
         <v>0.1</v>
       </c>
       <c r="E20" t="n">
-        <v>55.8</v>
+        <v>29.03333333333335</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>46.33333333333333</v>
+        <v>73.09999999999999</v>
       </c>
       <c r="B21" t="n">
         <v>0.1</v>
@@ -797,12 +797,12 @@
         <v>0.1</v>
       </c>
       <c r="E21" t="n">
-        <v>53.36666666666667</v>
+        <v>26.60000000000002</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>48.76666666666667</v>
+        <v>75.53333333333333</v>
       </c>
       <c r="B22" t="n">
         <v>0.1</v>
@@ -814,12 +814,12 @@
         <v>0.1</v>
       </c>
       <c r="E22" t="n">
-        <v>50.93333333333333</v>
+        <v>24.16666666666669</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>51.2</v>
+        <v>77.96666666666667</v>
       </c>
       <c r="B23" t="n">
         <v>0.1</v>
@@ -831,12 +831,12 @@
         <v>0.1</v>
       </c>
       <c r="E23" t="n">
-        <v>48.49999999999999</v>
+        <v>21.73333333333335</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>53.63333333333333</v>
+        <v>80.39999999999999</v>
       </c>
       <c r="B24" t="n">
         <v>0.1</v>
@@ -848,12 +848,12 @@
         <v>0.1</v>
       </c>
       <c r="E24" t="n">
-        <v>46.06666666666666</v>
+        <v>19.30000000000003</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>56.06666666666666</v>
+        <v>82.83333333333333</v>
       </c>
       <c r="B25" t="n">
         <v>0.1</v>
@@ -865,12 +865,12 @@
         <v>0.1</v>
       </c>
       <c r="E25" t="n">
-        <v>43.63333333333333</v>
+        <v>16.86666666666669</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>58.5</v>
+        <v>85.26666666666665</v>
       </c>
       <c r="B26" t="n">
         <v>0.1</v>
@@ -882,12 +882,12 @@
         <v>0.1</v>
       </c>
       <c r="E26" t="n">
-        <v>41.2</v>
+        <v>14.43333333333337</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>60.93333333333333</v>
+        <v>87.69999999999999</v>
       </c>
       <c r="B27" t="n">
         <v>0.1</v>
@@ -899,12 +899,12 @@
         <v>0.1</v>
       </c>
       <c r="E27" t="n">
-        <v>38.76666666666667</v>
+        <v>12.00000000000003</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>63.36666666666666</v>
+        <v>90.13333333333333</v>
       </c>
       <c r="B28" t="n">
         <v>0.1</v>
@@ -916,12 +916,12 @@
         <v>0.1</v>
       </c>
       <c r="E28" t="n">
-        <v>36.33333333333334</v>
+        <v>9.566666666666691</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>65.8</v>
+        <v>92.56666666666666</v>
       </c>
       <c r="B29" t="n">
         <v>0.1</v>
@@ -933,12 +933,12 @@
         <v>0.1</v>
       </c>
       <c r="E29" t="n">
-        <v>33.9</v>
+        <v>7.133333333333354</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>68.23333333333333</v>
+        <v>95</v>
       </c>
       <c r="B30" t="n">
         <v>0.1</v>
@@ -950,194 +950,7 @@
         <v>0.1</v>
       </c>
       <c r="E30" t="n">
-        <v>31.46666666666666</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="n">
-        <v>70.66666666666667</v>
-      </c>
-      <c r="B31" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="C31" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="D31" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="E31" t="n">
-        <v>29.03333333333332</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="n">
-        <v>73.09999999999999</v>
-      </c>
-      <c r="B32" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="C32" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="D32" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="E32" t="n">
-        <v>26.6</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="n">
-        <v>75.53333333333333</v>
-      </c>
-      <c r="B33" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="C33" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="D33" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="E33" t="n">
-        <v>24.16666666666666</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="n">
-        <v>77.96666666666667</v>
-      </c>
-      <c r="B34" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="C34" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="D34" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="E34" t="n">
-        <v>21.73333333333333</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="n">
-        <v>80.39999999999999</v>
-      </c>
-      <c r="B35" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="C35" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="D35" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="E35" t="n">
-        <v>19.3</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="n">
-        <v>82.83333333333333</v>
-      </c>
-      <c r="B36" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="C36" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="D36" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="E36" t="n">
-        <v>16.86666666666667</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="n">
-        <v>85.26666666666665</v>
-      </c>
-      <c r="B37" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="C37" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="D37" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="E37" t="n">
-        <v>14.43333333333335</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="n">
-        <v>87.69999999999999</v>
-      </c>
-      <c r="B38" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="C38" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="D38" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="E38" t="n">
-        <v>12.00000000000001</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="n">
-        <v>90.13333333333333</v>
-      </c>
-      <c r="B39" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="C39" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="D39" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="E39" t="n">
-        <v>9.566666666666675</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="n">
-        <v>92.56666666666666</v>
-      </c>
-      <c r="B40" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="C40" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="D40" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="E40" t="n">
-        <v>7.133333333333338</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="n">
-        <v>95</v>
-      </c>
-      <c r="B41" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="C41" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="D41" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="E41" t="n">
-        <v>4.700000000000001</v>
+        <v>4.700000000000017</v>
       </c>
     </row>
   </sheetData>

</xml_diff>